<commit_message>
update Cage RoleAndPermission file
</commit_message>
<xml_diff>
--- a/role_permission_files/Cage_RoleAndPermission.xlsx
+++ b/role_permission_files/Cage_RoleAndPermission.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="162">
   <si>
     <t>Version</t>
   </si>
@@ -418,9 +418,6 @@
     <t/>
   </si>
   <si>
-    <t>create</t>
-  </si>
-  <si>
     <t>player</t>
   </si>
   <si>
@@ -508,10 +505,40 @@
     <t>marketing_counter</t>
   </si>
   <si>
-    <t>it_specialist</t>
-  </si>
-  <si>
     <t>unlock</t>
+  </si>
+  <si>
+    <t>internal_external_role</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>sw_team</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>add_credit</t>
+  </si>
+  <si>
+    <t>y:1000</t>
+  </si>
+  <si>
+    <t>y:50000</t>
+  </si>
+  <si>
+    <t>expire_credit</t>
+  </si>
+  <si>
+    <t>lock_player_log</t>
+  </si>
+  <si>
+    <t>change_history</t>
+  </si>
+  <si>
+    <t>pin_change_log</t>
   </si>
 </sst>
 </file>
@@ -887,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1028,12 +1055,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1044,42 +1065,33 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1098,18 +1110,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1118,15 +1139,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1423,12 +1435,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
@@ -1572,16 +1584,16 @@
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" s="4">
         <v>42317</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
@@ -1885,157 +1897,157 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="59"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="53"/>
+      <c r="D4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="51"/>
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63"/>
-      <c r="B5" s="53" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="53"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="51"/>
     </row>
     <row r="6" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
-      <c r="B6" s="53" t="s">
+      <c r="A6" s="58"/>
+      <c r="B6" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="53"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
-      <c r="B7" s="53" t="s">
+      <c r="A7" s="58"/>
+      <c r="B7" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="53"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="51"/>
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="53"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="51"/>
     </row>
     <row r="9" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="64" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="44" t="s">
@@ -2054,11 +2066,11 @@
       <c r="I9" s="46"/>
     </row>
     <row r="10" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="70"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="44" t="s">
         <v>11</v>
       </c>
@@ -2075,11 +2087,11 @@
       <c r="I10" s="46"/>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="70"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="44" t="s">
         <v>11</v>
       </c>
@@ -2090,11 +2102,11 @@
       <c r="I11" s="46"/>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="44" t="s">
         <v>11</v>
       </c>
@@ -2111,11 +2123,11 @@
       <c r="I12" s="46"/>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="65"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="70"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="44" t="s">
         <v>11</v>
       </c>
@@ -2130,11 +2142,11 @@
       <c r="I13" s="46"/>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="65"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="70"/>
+      <c r="C14" s="65"/>
       <c r="D14" s="44" t="s">
         <v>11</v>
       </c>
@@ -2151,41 +2163,41 @@
       <c r="I14" s="46"/>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="65"/>
-      <c r="B15" s="52" t="s">
+      <c r="A15" s="60"/>
+      <c r="B15" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="65"/>
+      <c r="D15" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="45"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="46"/>
+    </row>
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="60"/>
+      <c r="B16" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="46"/>
-    </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65"/>
-      <c r="B16" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="52" t="s">
+      <c r="C16" s="65"/>
+      <c r="D16" s="50" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="45"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="46"/>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="71"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="44" t="s">
         <v>11</v>
       </c>
@@ -2200,11 +2212,11 @@
       <c r="I17" s="46"/>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="42"/>
-      <c r="C18" s="64" t="s">
+      <c r="C18" s="59" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="42" t="s">
@@ -2219,11 +2231,11 @@
       <c r="I18" s="43"/>
     </row>
     <row r="19" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
+      <c r="A19" s="59"/>
       <c r="B19" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="64"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="42" t="s">
         <v>11</v>
       </c>
@@ -2238,11 +2250,11 @@
       <c r="I19" s="43"/>
     </row>
     <row r="20" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="64"/>
+      <c r="C20" s="59"/>
       <c r="D20" s="43" t="s">
         <v>11</v>
       </c>
@@ -2276,127 +2288,127 @@
       <c r="I21" s="47"/>
     </row>
     <row r="22" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57" t="s">
+      <c r="D22" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="57" t="s">
+      <c r="A23" s="57"/>
+      <c r="B23" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57" t="s">
+      <c r="C23" s="57"/>
+      <c r="D23" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
-      <c r="B24" s="57" t="s">
+      <c r="A24" s="57"/>
+      <c r="B24" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57" t="s">
+      <c r="C24" s="57"/>
+      <c r="D24" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
-      <c r="B25" s="57" t="s">
+      <c r="A25" s="57"/>
+      <c r="B25" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57" t="s">
+      <c r="D25" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" s="57" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57" t="s">
+      <c r="C26" s="57"/>
+      <c r="D26" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="57" t="s">
+      <c r="A27" s="57"/>
+      <c r="B27" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57" t="s">
+      <c r="C27" s="57"/>
+      <c r="D27" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
-      <c r="B28" s="57" t="s">
+      <c r="A28" s="57"/>
+      <c r="B28" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57" t="s">
+      <c r="C28" s="57"/>
+      <c r="D28" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2503,7 +2515,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2518,550 +2530,537 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C2" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E2" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F2" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G2" s="52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="41" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="60"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="49"/>
+      <c r="C4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="49"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="49"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="55"/>
-      <c r="G8" s="46"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="55"/>
-      <c r="G9" s="46"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="46"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="55"/>
-      <c r="G11" s="46"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="55"/>
-      <c r="G12" s="46"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="55"/>
-      <c r="G13" s="46"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="46"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="46"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="46"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="54"/>
-      <c r="G17" s="43"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="C21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="A22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="A23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -3319,10 +3318,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="77"/>
+      <c r="B2" s="75"/>
       <c r="C2" s="28" t="s">
         <v>9</v>
       </c>
@@ -3349,16 +3348,16 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="68" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="73" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="34" t="s">
@@ -3375,12 +3374,12 @@
       <c r="L3" s="38"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="75"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="30" t="s">
         <v>11</v>
       </c>
@@ -3395,12 +3394,12 @@
       <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="75"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="30" t="s">
         <v>11</v>
       </c>
@@ -3415,12 +3414,12 @@
       <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="75"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="30" t="s">
         <v>11</v>
       </c>
@@ -3435,12 +3434,12 @@
       <c r="L6" s="30"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="75"/>
+      <c r="D7" s="71"/>
       <c r="E7" s="30" t="s">
         <v>11</v>
       </c>
@@ -3453,12 +3452,12 @@
       <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="75"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="30" t="s">
         <v>11</v>
       </c>
@@ -3509,10 +3508,10 @@
       <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="78" t="s">
+      <c r="B13" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="78"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="17" t="s">
         <v>9</v>
       </c>
@@ -3540,16 +3539,16 @@
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="67" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="80" t="s">
+      <c r="E14" s="69" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="33" t="s">
@@ -3568,15 +3567,15 @@
       <c r="M14" s="26"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="75" t="s">
+      <c r="A15" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="80"/>
+      <c r="E15" s="69"/>
       <c r="F15" s="15" t="s">
         <v>11</v>
       </c>
@@ -3593,13 +3592,13 @@
       <c r="M15" s="18"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="75"/>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="80"/>
+      <c r="E16" s="69"/>
       <c r="F16" s="15" t="s">
         <v>11</v>
       </c>
@@ -3616,13 +3615,13 @@
       <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="67"/>
       <c r="D17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="80"/>
+      <c r="E17" s="69"/>
       <c r="F17" s="15" t="s">
         <v>11</v>
       </c>
@@ -3639,13 +3638,13 @@
       <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="80"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="15" t="s">
         <v>11</v>
       </c>
@@ -3660,13 +3659,13 @@
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="75"/>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
       <c r="D19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="80"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="15" t="s">
         <v>11</v>
       </c>
@@ -3681,15 +3680,15 @@
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="80"/>
+      <c r="E20" s="69"/>
       <c r="F20" s="15" t="s">
         <v>11</v>
       </c>
@@ -3704,13 +3703,13 @@
       <c r="M20" s="25"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
-      <c r="B21" s="79"/>
-      <c r="C21" s="79"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
       <c r="D21" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="80"/>
+      <c r="E21" s="69"/>
       <c r="F21" s="15" t="s">
         <v>11</v>
       </c>
@@ -3725,13 +3724,13 @@
       <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="75"/>
-      <c r="B22" s="79"/>
-      <c r="C22" s="79"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
       <c r="D22" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="80"/>
+      <c r="E22" s="69"/>
       <c r="F22" s="15" t="s">
         <v>11</v>
       </c>
@@ -3746,13 +3745,13 @@
       <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="75"/>
-      <c r="B23" s="79"/>
-      <c r="C23" s="79"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
       <c r="D23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="80"/>
+      <c r="E23" s="69"/>
       <c r="F23" s="15" t="s">
         <v>11</v>
       </c>
@@ -3767,13 +3766,13 @@
       <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="75"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="80"/>
+      <c r="E24" s="69"/>
       <c r="F24" s="15" t="s">
         <v>11</v>
       </c>
@@ -3788,15 +3787,15 @@
       <c r="M24" s="25"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="75" t="s">
+      <c r="A25" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
       <c r="D25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="80"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="15" t="s">
         <v>11</v>
       </c>
@@ -3811,13 +3810,13 @@
       <c r="M25" s="25"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="75"/>
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
       <c r="D26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="80"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="15" t="s">
         <v>11</v>
       </c>
@@ -3832,13 +3831,13 @@
       <c r="M26" s="25"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="75"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
+      <c r="A27" s="71"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
       <c r="D27" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="80"/>
+      <c r="E27" s="69"/>
       <c r="F27" s="15" t="s">
         <v>11</v>
       </c>
@@ -3853,13 +3852,13 @@
       <c r="M27" s="25"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="75"/>
-      <c r="B28" s="79"/>
-      <c r="C28" s="79"/>
+      <c r="A28" s="71"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
       <c r="D28" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="80"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="15" t="s">
         <v>11</v>
       </c>
@@ -3874,13 +3873,13 @@
       <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="75"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
       <c r="D29" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="81"/>
+      <c r="E29" s="70"/>
       <c r="F29" s="15" t="s">
         <v>11</v>
       </c>
@@ -3923,17 +3922,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:B29"/>
     <mergeCell ref="C14:C29"/>
     <mergeCell ref="E14:E29"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3979,10 +3978,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="49" t="s">
         <v>63</v>
       </c>
       <c r="D3" t="s">

</xml_diff>